<commit_message>
epaper work, add font generator
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssacha\OneDrive\Робочий стіл\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ACTUAL\MINI_CLOCK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22456EB-6953-497C-953C-B9EF03FFC517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA18E932-BFFB-4D4A-A423-907B85F7A0F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>MPU6500</t>
   </si>
@@ -51,20 +51,50 @@
     <t>GPI</t>
   </si>
   <si>
-    <t>GPO</t>
-  </si>
-  <si>
     <t>IN</t>
   </si>
   <si>
-    <t>OUT</t>
+    <t>mini clock</t>
+  </si>
+  <si>
+    <t>AHT21</t>
+  </si>
+  <si>
+    <t>accel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LCD </t>
+  </si>
+  <si>
+    <t>OUT Enable</t>
+  </si>
+  <si>
+    <t>LCD</t>
+  </si>
+  <si>
+    <t>BUSY</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>ADC volt</t>
+  </si>
+  <si>
+    <t>INTR accel</t>
+  </si>
+  <si>
+    <t>RST</t>
+  </si>
+  <si>
+    <t>DC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,8 +123,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -104,6 +141,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -116,16 +158,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Гарний" xfId="2" builtinId="26"/>
     <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
     <cellStyle name="Колірна тема 1" xfId="1" builtinId="29"/>
   </cellStyles>
@@ -405,134 +452,219 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D18"/>
+  <dimension ref="C1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="F3" s="1"/>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
         <v>1</v>
       </c>
-      <c r="B5">
+      <c r="D5">
         <v>19</v>
       </c>
-      <c r="C5">
+      <c r="E5">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
         <v>2</v>
       </c>
-      <c r="B6">
+      <c r="D6">
         <v>23</v>
       </c>
-      <c r="C6">
+      <c r="E6">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8">
+      <c r="D8">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
         <v>7</v>
       </c>
-      <c r="B10">
+      <c r="D12">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
         <v>7</v>
       </c>
-      <c r="B11">
+      <c r="D13">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="14" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
         <v>7</v>
       </c>
-      <c r="B12">
+      <c r="D14">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="15" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
         <v>7</v>
       </c>
-      <c r="B13">
+      <c r="D15">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="16" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
         <v>7</v>
       </c>
-      <c r="B14">
+      <c r="D16">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16">
+      <c r="D21">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18">
-        <v>35</v>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>